<commit_message>
new results 15 aug 22
</commit_message>
<xml_diff>
--- a/code/fslstats_output/fslstats_output_12aug22_formatted.xlsx
+++ b/code/fslstats_output/fslstats_output_12aug22_formatted.xlsx
@@ -8,15 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/code/fslstats_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C89A09-3140-CE40-B200-DEC63EC13227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30FD26E-AC61-5F43-9F6A-EBCC05883A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fslstats_output_5aug22" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -1267,7 +1277,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1277,6 +1287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,12 +1309,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R103" sqref="R103"/>
+    <sheetView tabSelected="1" topLeftCell="M93" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J142" sqref="J142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1838,9 +1855,10 @@
       <c r="J8" t="s">
         <v>183</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="3" t="s">
         <v>225</v>
       </c>
+      <c r="N8" s="3"/>
       <c r="P8" t="s">
         <v>267</v>
       </c>
@@ -1870,10 +1888,10 @@
       <c r="K9">
         <v>0.25640000000000002</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
         <v>0.96779999999999999</v>
       </c>
       <c r="P9">
@@ -1951,10 +1969,10 @@
       <c r="G12" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="3"/>
       <c r="M12" t="s">
         <v>227</v>
       </c>
@@ -1981,10 +1999,10 @@
       <c r="H13">
         <v>0.77559999999999996</v>
       </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
         <v>0.99460000000000004</v>
       </c>
       <c r="M13">
@@ -2654,9 +2672,10 @@
       <c r="J36" t="s">
         <v>197</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="3" t="s">
         <v>239</v>
       </c>
+      <c r="N36" s="3"/>
       <c r="P36" t="s">
         <v>281</v>
       </c>
@@ -2686,10 +2705,10 @@
       <c r="K37">
         <v>0.17499999999999999</v>
       </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
         <v>0.96240000000000003</v>
       </c>
       <c r="P37">
@@ -2767,10 +2786,10 @@
       <c r="G40" t="s">
         <v>91</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="K40" s="2"/>
+      <c r="K40" s="3"/>
       <c r="M40" t="s">
         <v>241</v>
       </c>
@@ -2797,10 +2816,10 @@
       <c r="H41">
         <v>0.12859999999999999</v>
       </c>
-      <c r="J41" s="2">
-        <v>0</v>
-      </c>
-      <c r="K41" s="2">
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
         <v>0.98160000000000003</v>
       </c>
       <c r="M41">
@@ -3585,10 +3604,10 @@
       <c r="J68" t="s">
         <v>213</v>
       </c>
-      <c r="M68" s="2" t="s">
+      <c r="M68" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="N68" s="2"/>
+      <c r="N68" s="3"/>
       <c r="P68" t="s">
         <v>297</v>
       </c>
@@ -3618,10 +3637,10 @@
       <c r="K69">
         <v>0.80020000000000002</v>
       </c>
-      <c r="M69" s="2">
-        <v>0</v>
-      </c>
-      <c r="N69" s="2">
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+      <c r="N69" s="3">
         <v>0.96340000000000003</v>
       </c>
       <c r="P69">
@@ -3914,10 +3933,10 @@
       <c r="G80" t="s">
         <v>158</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J80" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="K80" s="2"/>
+      <c r="K80" s="3"/>
       <c r="M80" t="s">
         <v>261</v>
       </c>
@@ -3944,10 +3963,10 @@
       <c r="H81">
         <v>0.66339999999999999</v>
       </c>
-      <c r="J81" s="2">
-        <v>0</v>
-      </c>
-      <c r="K81" s="2">
+      <c r="J81" s="3">
+        <v>0</v>
+      </c>
+      <c r="K81" s="3">
         <v>0.97199999999999998</v>
       </c>
       <c r="M81">
@@ -4187,10 +4206,10 @@
       <c r="G90" t="s">
         <v>163</v>
       </c>
-      <c r="J90" s="2" t="s">
+      <c r="J90" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="K90" s="2"/>
+      <c r="K90" s="3"/>
       <c r="M90" t="s">
         <v>337</v>
       </c>
@@ -4217,10 +4236,10 @@
       <c r="H91">
         <v>0.65439999999999998</v>
       </c>
-      <c r="J91" s="2">
-        <v>0</v>
-      </c>
-      <c r="K91" s="2">
+      <c r="J91" s="3">
+        <v>0</v>
+      </c>
+      <c r="K91" s="3">
         <v>0.99639999999999995</v>
       </c>
       <c r="M91">
@@ -4770,10 +4789,10 @@
       <c r="G110" t="s">
         <v>173</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="J110" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="K110" s="2"/>
+      <c r="K110" s="3"/>
       <c r="M110" t="s">
         <v>347</v>
       </c>
@@ -4800,10 +4819,10 @@
       <c r="H111">
         <v>0.50980000000000003</v>
       </c>
-      <c r="J111" s="2">
-        <v>0</v>
-      </c>
-      <c r="K111" s="2">
+      <c r="J111" s="3">
+        <v>0</v>
+      </c>
+      <c r="K111" s="3">
         <v>0.98599999999999999</v>
       </c>
       <c r="M111">
@@ -5268,9 +5287,10 @@
       <c r="M130" t="s">
         <v>357</v>
       </c>
-      <c r="P130" t="s">
+      <c r="P130" s="3" t="s">
         <v>387</v>
       </c>
+      <c r="Q130" s="3"/>
     </row>
     <row r="131" spans="10:17" x14ac:dyDescent="0.15">
       <c r="J131">
@@ -5285,10 +5305,10 @@
       <c r="N131">
         <v>0.73260000000000003</v>
       </c>
-      <c r="P131">
-        <v>0</v>
-      </c>
-      <c r="Q131">
+      <c r="P131" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="3">
         <v>0.95479999999999998</v>
       </c>
     </row>

</xml_diff>